<commit_message>
Hub & StandardPharma file modified and split locators
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\PycharmProject\LegrandePython\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4529D91C-0409-49C4-BFBD-DD132E3F03C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C807CD95-9311-402F-A228-2A1B5D53F80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Credentials" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="86">
   <si>
     <t>Portal</t>
   </si>
@@ -66,9 +66,6 @@
     <t>https://ibis-dev.droicelabs.us/dispenser</t>
   </si>
   <si>
-    <t>monica.hub@mailinator.com</t>
-  </si>
-  <si>
     <t>RX Standard Pharma</t>
   </si>
   <si>
@@ -105,21 +102,6 @@
     <t>PatientName</t>
   </si>
   <si>
-    <t>PracticeName</t>
-  </si>
-  <si>
-    <t>Order Type</t>
-  </si>
-  <si>
-    <t>RX Product</t>
-  </si>
-  <si>
-    <t>OTC Product</t>
-  </si>
-  <si>
-    <t>Compound Product</t>
-  </si>
-  <si>
     <t>Product Instruction</t>
   </si>
   <si>
@@ -183,21 +165,6 @@
     <t>Kristina Vang (01/06/2022)</t>
   </si>
   <si>
-    <t>Diza</t>
-  </si>
-  <si>
-    <t>Onetime</t>
-  </si>
-  <si>
-    <t>100 Rx</t>
-  </si>
-  <si>
-    <t>100 OTC</t>
-  </si>
-  <si>
-    <t>100 Compound</t>
-  </si>
-  <si>
     <t>Follow this instructions.</t>
   </si>
   <si>
@@ -310,6 +277,9 @@
   </si>
   <si>
     <t>Visa **** **** **** 0026 (Expires 12/2049)*0783440aefbbfd60e24ec63344364d0d060e6f5087410066000000000000000000000000000000000000000030343952303337373034ffff9876540006800053404003</t>
+  </si>
+  <si>
+    <t>hub.vp@getnada.com</t>
   </si>
 </sst>
 </file>
@@ -386,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -401,6 +371,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,8 +715,8 @@
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
+      <c r="C4" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
@@ -753,13 +724,13 @@
     </row>
     <row r="5" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
@@ -767,13 +738,13 @@
     </row>
     <row r="6" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -781,13 +752,13 @@
     </row>
     <row r="7" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>11</v>
@@ -795,13 +766,13 @@
     </row>
     <row r="8" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>11</v>
@@ -809,13 +780,13 @@
     </row>
     <row r="9" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>11</v>
@@ -823,205 +794,171 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.88671875" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.77734375" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="19.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.77734375" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="49" width="26.109375" style="7" customWidth="1"/>
-    <col min="50" max="16384" width="26.109375" style="7"/>
+    <col min="3" max="3" width="23.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="19.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="44" width="26.109375" style="7" customWidth="1"/>
+    <col min="45" max="16384" width="26.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="6" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="6" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="U1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="2">
+        <v>123</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="K2" s="2">
+        <v>2025</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="P2" s="2">
+        <v>99835</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="T2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="N2" s="2">
-        <v>123</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="P2" s="2">
-        <v>2025</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="U2" s="2">
-        <v>99835</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y2" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z2" s="2">
         <v>35004</v>
       </c>
     </row>
@@ -1058,78 +995,78 @@
   <sheetData>
     <row r="1" spans="1:12" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="7" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>